<commit_message>
implémentation de la page d'accueil avec les annonces
</commit_message>
<xml_diff>
--- a/data/ads.xlsx
+++ b/data/ads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sellMyTools\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207DF6D4-16EF-4DCC-9D4C-5EE0A23AC334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA57494-0D16-48E3-B315-B4A369A76520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{84D11D7A-3AEC-4076-9CE2-7E81F7D4839D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -93,7 +93,10 @@
     <t>PUBLIE</t>
   </si>
   <si>
-    <t>perceuse.jfif</t>
+    <t>perceuse-01.jpg</t>
+  </si>
+  <si>
+    <t>perceuse-02.jpg</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,6 +492,8 @@
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -561,7 +566,7 @@
         <v>18</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L2" t="b">
         <v>1</v>
@@ -599,7 +604,7 @@
         <v>18</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L3" t="b">
         <v>0</v>

</xml_diff>